<commit_message>
Adds an up and down example of r1c1
</commit_message>
<xml_diff>
--- a/src/test/resources/r1c1.xlsx
+++ b/src/test/resources/r1c1.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -368,6 +368,12 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>AVERAGE(A1:A2)</f>
+        <v>4.5</v>
+      </c>
+    </row>
     <row r="9" spans="1:6">
       <c r="C9">
         <f>$C$1+$C$2</f>

</xml_diff>